<commit_message>
Moved app.py and render.yaml to root
</commit_message>
<xml_diff>
--- a/user_log_history.xlsx
+++ b/user_log_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -701,7 +701,33 @@
           <t>2025-07-12 12:35:40</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-07-12 16:07:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>kumarshashwat890@gmail.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Shashwat kumar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-07-12 16:07:47</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-07-12 16:09:06</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Moved app.py and all files to root
</commit_message>
<xml_diff>
--- a/user_log_history.xlsx
+++ b/user_log_history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -729,6 +729,24 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>kumarshashwat890@gmail.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Shashwat kumar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-07-12 17:10:01</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>